<commit_message>
Updated data.js to v10.18
</commit_message>
<xml_diff>
--- a/Excel Data/Kanban Pallet Weight List.xlsx
+++ b/Excel Data/Kanban Pallet Weight List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="684" documentId="11_F25DC773A252ABEACE02EC95335E46045BDE589C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{7369654D-38AE-43F8-961E-C2CA70F4DBAA}"/>
+  <xr:revisionPtr revIDLastSave="727" documentId="11_F25DC773A252ABEACE02EC95335E46045BDE589C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4890A61F-E844-4E98-87A3-5C87282B431C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="6735" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="144">
   <si>
     <t>Part Number</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>A1531658A0100</t>
-  </si>
-  <si>
-    <t>A5400700L0200</t>
   </si>
   <si>
     <t>A1540078L0200</t>
@@ -289,12 +286,6 @@
     <t>A2C7449700000</t>
   </si>
   <si>
-    <t>A2C7471630200</t>
-  </si>
-  <si>
-    <t>Trend Tech</t>
-  </si>
-  <si>
     <t>A2C7473260100</t>
   </si>
   <si>
@@ -403,9 +394,6 @@
     <t>A2C7363430200</t>
   </si>
   <si>
-    <t>A2C7471640200</t>
-  </si>
-  <si>
     <t>A2C7716160300</t>
   </si>
   <si>
@@ -443,6 +431,27 @@
   </si>
   <si>
     <t>A2C0153000000</t>
+  </si>
+  <si>
+    <t>A1540077L0200</t>
+  </si>
+  <si>
+    <t>A2C1039870000</t>
+  </si>
+  <si>
+    <t>A2C1836950000</t>
+  </si>
+  <si>
+    <t>A2C7600840000</t>
+  </si>
+  <si>
+    <t>A2C9175080000</t>
+  </si>
+  <si>
+    <t>A2C9137910000</t>
+  </si>
+  <si>
+    <t>FRK</t>
   </si>
 </sst>
 </file>
@@ -790,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S978"/>
+  <dimension ref="A1:S981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection sqref="A1:E114"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E117" sqref="A1:E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,13 +1130,13 @@
         <v>9242500089000</v>
       </c>
       <c r="C11" s="1">
-        <v>1440</v>
+        <v>2160</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1">
-        <v>340</v>
+        <v>510</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1242,7 +1251,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="C15" s="1">
         <v>900</v>
@@ -1273,7 +1282,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1">
         <v>720</v>
@@ -1304,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1">
         <v>351</v>
@@ -1335,7 +1344,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1">
         <v>300</v>
@@ -1366,13 +1375,13 @@
         <v>0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1">
         <v>720</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1">
         <v>300</v>
@@ -1397,13 +1406,13 @@
         <v>0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1">
         <v>400</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1">
         <v>800</v>
@@ -1428,13 +1437,13 @@
         <v>0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1">
         <v>360</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="1">
         <v>500</v>
@@ -1459,13 +1468,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1">
         <v>360</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1">
         <v>600</v>
@@ -1490,13 +1499,13 @@
         <v>0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1">
         <v>672</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" s="1">
         <v>600</v>
@@ -1521,16 +1530,16 @@
         <v>0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1">
-        <v>960</v>
+        <v>144</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="E24" s="1">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1552,16 +1561,16 @@
         <v>0</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>133</v>
+        <v>30</v>
       </c>
       <c r="C25" s="1">
-        <v>960</v>
+        <v>360</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="E25" s="1">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1583,13 +1592,13 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C26" s="1">
         <v>960</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E26" s="1">
         <v>450</v>
@@ -1614,16 +1623,16 @@
         <v>0</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
       <c r="C27" s="1">
-        <v>144</v>
+        <v>960</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="E27" s="1">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1645,25 +1654,20 @@
         <v>0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="C28" s="1">
-        <v>360</v>
+        <v>960</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="E28" s="1">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1676,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C29" s="1">
         <v>264</v>
@@ -1690,11 +1694,6 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -1706,17 +1705,17 @@
       <c r="A30" s="1">
         <v>0</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>123</v>
+      <c r="B30" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="C30" s="1">
-        <v>4032</v>
+        <v>648</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="E30" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1737,17 +1736,17 @@
       <c r="A31" s="1">
         <v>0</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="1">
-        <v>4800</v>
+      <c r="B31" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2304</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="E31" s="1">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1769,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C32" s="1">
         <v>4032</v>
@@ -1778,7 +1777,7 @@
         <v>6</v>
       </c>
       <c r="E32" s="1">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1797,19 +1796,19 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C33" s="1">
-        <v>520</v>
+        <v>4800</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E33" s="1">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1828,19 +1827,19 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="C34" s="1">
-        <v>0</v>
+        <v>4032</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E34" s="1">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -1859,19 +1858,19 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35" s="1">
-        <v>1200</v>
+        <v>520</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E35" s="1">
-        <v>600</v>
+        <v>450</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1890,19 +1889,19 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="1">
         <v>0</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="1">
-        <v>396</v>
-      </c>
       <c r="D36" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E36" s="1">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -1924,16 +1923,16 @@
         <v>0</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C37" s="1">
-        <v>18144</v>
+        <v>1200</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E37" s="1">
-        <v>1100</v>
+        <v>600</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1955,16 +1954,16 @@
         <v>0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C38" s="1">
-        <v>1280</v>
+        <v>396</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E38" s="1">
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1986,16 +1985,16 @@
         <v>0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C39" s="1">
-        <v>640</v>
+        <v>18144</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="E39" s="1">
-        <v>1050</v>
+        <v>1100</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -2017,16 +2016,16 @@
         <v>0</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C40" s="1">
-        <v>3276</v>
+        <v>1280</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E40" s="1">
-        <v>620</v>
+        <v>420</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2048,16 +2047,16 @@
         <v>0</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C41" s="1">
-        <v>3276</v>
+        <v>640</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="E41" s="1">
-        <v>620</v>
+        <v>1050</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -2079,13 +2078,13 @@
         <v>0</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C42" s="1">
         <v>3276</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E42" s="1">
         <v>620</v>
@@ -2110,16 +2109,16 @@
         <v>0</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C43" s="1">
-        <v>1440</v>
+        <v>3276</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E43" s="1">
-        <v>350</v>
+        <v>620</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -2141,16 +2140,16 @@
         <v>0</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="C44" s="1">
-        <v>1728</v>
+        <v>3276</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E44" s="1">
-        <v>300</v>
+        <v>620</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -2172,16 +2171,16 @@
         <v>0</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C45" s="1">
-        <v>4800</v>
+        <v>1440</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E45" s="1">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -2203,16 +2202,16 @@
         <v>0</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="C46" s="1">
-        <v>11520</v>
+        <v>1728</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E46" s="1">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -2234,16 +2233,16 @@
         <v>0</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C47" s="1">
-        <v>3600</v>
+        <v>4800</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="E47" s="1">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -2265,16 +2264,16 @@
         <v>0</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C48" s="1">
-        <v>3600</v>
+        <v>11520</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E48" s="1">
-        <v>450</v>
+        <v>350</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -2295,17 +2294,17 @@
       <c r="A49" s="1">
         <v>0</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>54</v>
+      <c r="B49" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C49" s="1">
-        <v>576</v>
+        <v>3600</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E49" s="1">
-        <v>300</v>
+        <v>450</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2324,19 +2323,19 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>1</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>56</v>
+        <v>0</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C50" s="1">
-        <v>384</v>
+        <v>3600</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="E50" s="1">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -2355,19 +2354,19 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C51" s="1">
-        <v>720</v>
+        <v>576</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E51" s="1">
-        <v>740</v>
+        <v>300</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -2386,19 +2385,19 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>134</v>
+        <v>55</v>
       </c>
       <c r="C52" s="1">
-        <v>576</v>
+        <v>384</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="E52" s="1">
-        <v>340</v>
+        <v>400</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2417,19 +2416,19 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C53" s="1">
-        <v>1440</v>
+        <v>720</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E53" s="1">
-        <v>350</v>
+        <v>740</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -2451,16 +2450,16 @@
         <v>0</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="C54" s="1">
-        <v>1760</v>
+        <v>576</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="E54" s="1">
-        <v>700</v>
+        <v>340</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -2482,16 +2481,16 @@
         <v>0</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C55" s="1">
-        <v>3600</v>
+        <v>1440</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E55" s="1">
-        <v>450</v>
+        <v>350</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2513,16 +2512,16 @@
         <v>0</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C56" s="1">
-        <v>2520</v>
+        <v>1760</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E56" s="1">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -2544,16 +2543,16 @@
         <v>0</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C57" s="1">
-        <v>1296</v>
+        <v>3600</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E57" s="1">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -2575,16 +2574,16 @@
         <v>0</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1">
-        <v>420</v>
+        <v>2520</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E58" s="1">
-        <v>950</v>
+        <v>400</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -2606,16 +2605,16 @@
         <v>0</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>126</v>
+        <v>63</v>
       </c>
       <c r="C59" s="1">
-        <v>1680</v>
+        <v>1296</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E59" s="1">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -2637,16 +2636,16 @@
         <v>0</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C60" s="1">
-        <v>240</v>
+        <v>420</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E60" s="1">
-        <v>300</v>
+        <v>950</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -2668,16 +2667,16 @@
         <v>0</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="C61" s="1">
-        <v>990</v>
+        <v>1680</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="E61" s="1">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -2696,19 +2695,19 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C62" s="1">
-        <v>384</v>
+        <v>240</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E62" s="1">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -2727,19 +2726,19 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C63" s="1">
-        <v>520</v>
+        <v>990</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E63" s="1">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -2758,19 +2757,19 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C64" s="1">
-        <v>192</v>
+        <v>384</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E64" s="1">
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -2789,19 +2788,19 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C65" s="1">
-        <v>396</v>
+        <v>520</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E65" s="1">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -2823,16 +2822,16 @@
         <v>0</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C66" s="1">
-        <v>800</v>
+        <v>192</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E66" s="1">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -2854,16 +2853,16 @@
         <v>0</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="C67" s="1">
-        <v>7560</v>
+        <v>396</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E67" s="1">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -2885,16 +2884,16 @@
         <v>0</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>136</v>
+        <v>71</v>
       </c>
       <c r="C68" s="1">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
       <c r="E68" s="1">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -2916,16 +2915,16 @@
         <v>0</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="C69" s="1">
-        <v>1440</v>
+        <v>7560</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E69" s="1">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -2947,16 +2946,16 @@
         <v>0</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="C70" s="1">
-        <v>8400</v>
+        <v>500</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>9</v>
+        <v>133</v>
       </c>
       <c r="E70" s="1">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -2978,16 +2977,16 @@
         <v>0</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C71" s="1">
-        <v>10500</v>
+        <v>1440</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E71" s="1">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -3006,19 +3005,19 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C72" s="1">
-        <v>1632</v>
+        <v>8400</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E72" s="1">
-        <v>520</v>
+        <v>700</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -3037,19 +3036,19 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C73" s="1">
-        <v>1280</v>
+        <v>10500</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="E73" s="1">
-        <v>420</v>
+        <v>500</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -3071,16 +3070,16 @@
         <v>1</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C74" s="1">
-        <v>1900</v>
+        <v>1632</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E74" s="1">
-        <v>1650</v>
+        <v>520</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -3102,16 +3101,16 @@
         <v>1</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C75" s="1">
-        <v>2160</v>
+        <v>1280</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E75" s="1">
-        <v>1450</v>
+        <v>420</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -3130,19 +3129,19 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C76" s="1">
-        <v>420</v>
+        <v>1900</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="E76" s="1">
-        <v>550</v>
+        <v>1650</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -3161,19 +3160,19 @@
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C77" s="1">
-        <v>1344</v>
+        <v>2160</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="E77" s="1">
-        <v>400</v>
+        <v>1450</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -3195,16 +3194,16 @@
         <v>0</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C78" s="1">
-        <v>2736</v>
+        <v>420</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E78" s="1">
-        <v>250</v>
+        <v>550</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -3226,16 +3225,16 @@
         <v>0</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C79" s="1">
-        <v>4212</v>
+        <v>1344</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="E79" s="1">
-        <v>475</v>
+        <v>400</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -3257,16 +3256,16 @@
         <v>0</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C80" s="1">
-        <v>4212</v>
+        <v>2736</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="E80" s="1">
-        <v>475</v>
+        <v>250</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -3288,16 +3287,16 @@
         <v>0</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C81" s="1">
-        <v>1440</v>
+        <v>4212</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E81" s="1">
-        <v>300</v>
+        <v>475</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -3319,21 +3318,21 @@
         <v>0</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C82" s="1">
-        <v>3600</v>
+        <v>4212</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="E82" s="1">
-        <v>450</v>
+        <v>475</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
-      <c r="I82" s="5"/>
+      <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
@@ -3350,16 +3349,16 @@
         <v>0</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C83" s="1">
-        <v>3600</v>
+        <v>1440</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E83" s="1">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
@@ -3381,21 +3380,21 @@
         <v>0</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C84" s="1">
-        <v>960</v>
+        <v>3600</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="E84" s="1">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
+      <c r="I84" s="5"/>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
@@ -3412,16 +3411,16 @@
         <v>0</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="C85" s="1">
-        <v>960</v>
+        <v>3600</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="E85" s="1">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -3443,13 +3442,13 @@
         <v>0</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C86" s="1">
         <v>432</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E86" s="1">
         <v>250</v>
@@ -3474,13 +3473,13 @@
         <v>0</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C87" s="1">
         <v>1800</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E87" s="1">
         <v>400</v>
@@ -3505,13 +3504,13 @@
         <v>0</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C88" s="1">
         <v>1800</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E88" s="1">
         <v>450</v>
@@ -3536,7 +3535,7 @@
         <v>1</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C89" s="1">
         <v>255</v>
@@ -3567,13 +3566,13 @@
         <v>1</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C90" s="1">
         <v>576</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E90" s="1">
         <v>450</v>
@@ -3598,13 +3597,13 @@
         <v>0</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C91" s="1">
         <v>576</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E91" s="1">
         <v>275</v>
@@ -3629,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C92" s="1">
         <v>180</v>
@@ -3660,13 +3659,13 @@
         <v>0</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C93" s="1">
         <v>3276</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E93" s="1">
         <v>620</v>
@@ -3691,13 +3690,13 @@
         <v>0</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C94" s="1">
         <v>3276</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E94" s="1">
         <v>620</v>
@@ -3722,13 +3721,13 @@
         <v>0</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C95" s="1">
         <v>408</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E95" s="1">
         <v>350</v>
@@ -3753,7 +3752,7 @@
         <v>0</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C96" s="1">
         <v>312</v>
@@ -3784,13 +3783,13 @@
         <v>0</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C97" s="1">
         <v>180</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E97" s="1">
         <v>700</v>
@@ -3815,13 +3814,13 @@
         <v>0</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C98" s="1">
         <v>600</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E98" s="1">
         <v>500</v>
@@ -3846,13 +3845,13 @@
         <v>0</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C99" s="1">
         <v>336</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E99" s="1">
         <v>125</v>
@@ -3877,13 +3876,13 @@
         <v>0</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C100" s="1">
         <v>336</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E100" s="1">
         <v>125</v>
@@ -3908,13 +3907,13 @@
         <v>0</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C101" s="1">
         <v>528</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E101" s="1">
         <v>350</v>
@@ -3939,13 +3938,13 @@
         <v>0</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="C102" s="1">
         <v>1872</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E102" s="1">
         <v>400</v>
@@ -3970,16 +3969,16 @@
         <v>0</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C103" s="1">
-        <v>960</v>
+        <v>1872</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="E103" s="1">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
@@ -4001,16 +4000,16 @@
         <v>0</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C104" s="1">
-        <v>660</v>
+        <v>960</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="E104" s="1">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
@@ -4032,13 +4031,13 @@
         <v>0</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C105" s="1">
-        <v>2376</v>
+        <v>660</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E105" s="1">
         <v>500</v>
@@ -4063,16 +4062,16 @@
         <v>0</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C106" s="1">
-        <v>240</v>
+        <v>2376</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="E106" s="1">
-        <v>80</v>
+        <v>500</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
@@ -4094,13 +4093,13 @@
         <v>0</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C107" s="1">
         <v>240</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E107" s="1">
         <v>80</v>
@@ -4125,16 +4124,16 @@
         <v>0</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="C108" s="1">
-        <v>4800</v>
+        <v>240</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="E108" s="1">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
@@ -4156,16 +4155,16 @@
         <v>0</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C109" s="1">
-        <v>15600</v>
+        <v>4800</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>115</v>
+        <v>31</v>
       </c>
       <c r="E109" s="1">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
@@ -4187,16 +4186,16 @@
         <v>0</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="C110" s="1">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="E110" s="1">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
@@ -4218,16 +4217,16 @@
         <v>0</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="C111" s="1">
-        <v>768</v>
+        <v>840</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="E111" s="1">
-        <v>650</v>
+        <v>200</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
@@ -4249,16 +4248,16 @@
         <v>0</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C112" s="1">
-        <v>1280</v>
+        <v>15600</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="E112" s="1">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
@@ -4277,19 +4276,19 @@
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C113" s="1">
-        <v>960</v>
+        <v>192</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E113" s="1">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
@@ -4308,19 +4307,19 @@
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C114" s="1">
-        <v>1280</v>
+        <v>768</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="E114" s="1">
-        <v>420</v>
+        <v>650</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
@@ -4338,6 +4337,21 @@
       <c r="S114" s="1"/>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>0</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C115" s="1">
+        <v>1280</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E115" s="1">
+        <v>400</v>
+      </c>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
@@ -4354,6 +4368,21 @@
       <c r="S115" s="1"/>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>1</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C116" s="1">
+        <v>960</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E116" s="1">
+        <v>380</v>
+      </c>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
@@ -4370,11 +4399,21 @@
       <c r="S116" s="1"/>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
+      <c r="A117" s="1">
+        <v>1</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C117" s="1">
+        <v>1280</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E117" s="1">
+        <v>420</v>
+      </c>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
@@ -4391,11 +4430,6 @@
       <c r="S117" s="1"/>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
-      <c r="B118" s="2"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
@@ -4412,11 +4446,6 @@
       <c r="S118" s="1"/>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
@@ -22471,6 +22500,69 @@
       <c r="R978" s="1"/>
       <c r="S978" s="1"/>
     </row>
+    <row r="979" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A979" s="1"/>
+      <c r="B979" s="2"/>
+      <c r="C979" s="1"/>
+      <c r="D979" s="1"/>
+      <c r="E979" s="1"/>
+      <c r="F979" s="1"/>
+      <c r="G979" s="1"/>
+      <c r="H979" s="1"/>
+      <c r="I979" s="1"/>
+      <c r="J979" s="1"/>
+      <c r="K979" s="1"/>
+      <c r="L979" s="1"/>
+      <c r="M979" s="1"/>
+      <c r="N979" s="1"/>
+      <c r="O979" s="1"/>
+      <c r="P979" s="1"/>
+      <c r="Q979" s="1"/>
+      <c r="R979" s="1"/>
+      <c r="S979" s="1"/>
+    </row>
+    <row r="980" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A980" s="1"/>
+      <c r="B980" s="2"/>
+      <c r="C980" s="1"/>
+      <c r="D980" s="1"/>
+      <c r="E980" s="1"/>
+      <c r="F980" s="1"/>
+      <c r="G980" s="1"/>
+      <c r="H980" s="1"/>
+      <c r="I980" s="1"/>
+      <c r="J980" s="1"/>
+      <c r="K980" s="1"/>
+      <c r="L980" s="1"/>
+      <c r="M980" s="1"/>
+      <c r="N980" s="1"/>
+      <c r="O980" s="1"/>
+      <c r="P980" s="1"/>
+      <c r="Q980" s="1"/>
+      <c r="R980" s="1"/>
+      <c r="S980" s="1"/>
+    </row>
+    <row r="981" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A981" s="1"/>
+      <c r="B981" s="2"/>
+      <c r="C981" s="1"/>
+      <c r="D981" s="1"/>
+      <c r="E981" s="1"/>
+      <c r="F981" s="1"/>
+      <c r="G981" s="1"/>
+      <c r="H981" s="1"/>
+      <c r="I981" s="1"/>
+      <c r="J981" s="1"/>
+      <c r="K981" s="1"/>
+      <c r="L981" s="1"/>
+      <c r="M981" s="1"/>
+      <c r="N981" s="1"/>
+      <c r="O981" s="1"/>
+      <c r="P981" s="1"/>
+      <c r="Q981" s="1"/>
+      <c r="R981" s="1"/>
+      <c r="S981" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>